<commit_message>
Added files with o1-preview reasoning, added new file for testing w/ o1-preview reasoning
</commit_message>
<xml_diff>
--- a/data/gpqa_diamond_15.xlsx
+++ b/data/gpqa_diamond_15.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Custom-LLM\laboratory-scale-ai\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Custom-LLM-AWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4242F7C3-1A60-44BA-98B4-2D14660BC1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE7FF9E4-5CF6-4DF5-8D1D-C929D1E6B1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900"/>
   </bookViews>
@@ -1025,7 +1025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="387.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>